<commit_message>
Update annotations for paris
</commit_message>
<xml_diff>
--- a/annotations/paris_20240724_172753.xlsx
+++ b/annotations/paris_20240724_172753.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,57 @@
           <t>issue_type</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>source_file</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>paris</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>APC</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>RES</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1269f1fb-9c21-42a9-ae5e-c80f92622adc</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Bk6qQGWRb_annotated.xlsx</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Then how bootstrap dqn extend the idea to deep learning, followed by the noisy net, bbq, shallow UBE and LS-DQN.</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>